<commit_message>
Se reemplazaron graficas circulares por gr[aficas de columna.
</commit_message>
<xml_diff>
--- a/Prueba/UrgenciaPorCausayEdad.xlsx
+++ b/Prueba/UrgenciaPorCausayEdad.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8688ca3d1d320028/Escritorio/Universidad/Semestre 10/rstudio/repositorio-de-prueba/Prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{8E0FDDD9-090C-43F3-AE8A-693F2208E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{657E31F6-DBB0-4C28-A3CC-A1EB57B6E4F7}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{8E0FDDD9-090C-43F3-AE8A-693F2208E5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A09E647F-8370-48CB-B8CB-08C9FCD6C5BA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB2892A7-5079-4099-98C4-30A44261E59B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DB2892A7-5079-4099-98C4-30A44261E59B}"/>
   </bookViews>
   <sheets>
     <sheet name="Causa" sheetId="1" r:id="rId1"/>
-    <sheet name="Edad" sheetId="2" r:id="rId2"/>
+    <sheet name="Causa2" sheetId="3" r:id="rId2"/>
+    <sheet name="Edad" sheetId="2" r:id="rId3"/>
+    <sheet name="Edad2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
   <si>
     <t>TOTAL</t>
   </si>
@@ -76,13 +78,25 @@
   </si>
   <si>
     <t>Adultos de 65 y más años</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Tipo de causa</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Edad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +141,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -142,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -189,11 +209,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -210,6 +245,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1793F3E4-4372-49D4-89C7-F816561630E4}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,11 +738,261 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C754421-7BE5-4E39-A8BD-F367632A37D4}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11">
+        <v>14398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>15751</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11">
+        <v>39423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11">
+        <v>4035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11">
+        <v>8832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11">
+        <v>24317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="11">
+        <v>8204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11">
+        <v>23358</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12">
+        <v>11428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="12">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="12">
+        <v>9342</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12">
+        <v>26820</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C1C692-9E52-49E0-AEE6-01F190CE44E9}">
   <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,4 +1146,254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AA8737-B7B5-4971-A8BC-A2F804E5BFC1}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11">
+        <v>9837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11">
+        <v>12054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11">
+        <v>34678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="11">
+        <v>12825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14">
+        <v>25531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="14">
+        <v>9568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11">
+        <v>4920</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11">
+        <v>23154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="11">
+        <v>9408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="14">
+        <v>3429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="14">
+        <v>9244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="14">
+        <v>9911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="14">
+        <v>21519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="14">
+        <v>9260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>